<commit_message>
Included code and "Submissions" for Bera_2011
</commit_message>
<xml_diff>
--- a/in-progress/Bera_2011_TActa/Bera_2011_TActa_Tidy_Table.xlsx
+++ b/in-progress/Bera_2011_TActa/Bera_2011_TActa_Tidy_Table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harrisondavis/Documents/GitHub/nmcuration/wishlist/Bera_2011_TActa/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harrisondavis/Documents/GitHub/nmcuration/in-progress/Bera_2011_TActa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE6DB17-D4C6-6F4F-9AF3-E3F6F2D6E9D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDCFB88-4F6C-A64C-AF1B-105398D4200C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="460" windowWidth="21840" windowHeight="17540" xr2:uid="{30166B8E-BF36-4C4B-B61F-0D57A7E70461}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21840" windowHeight="17540" xr2:uid="{30166B8E-BF36-4C4B-B61F-0D57A7E70461}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,21 +38,6 @@
     <t>Sample</t>
   </si>
   <si>
-    <t>Onset Temp (˚C)</t>
-  </si>
-  <si>
-    <t>Weight Loss @ Onset Temp (%)</t>
-  </si>
-  <si>
-    <t>DTG Max (˚C)</t>
-  </si>
-  <si>
-    <t>Non-Volatile Residue (%)</t>
-  </si>
-  <si>
-    <t>Sample (PS+X wt% silica)</t>
-  </si>
-  <si>
     <t>S1</t>
   </si>
   <si>
@@ -71,9 +56,6 @@
     <t>S6</t>
   </si>
   <si>
-    <t>Glass Transition Temp. T(g) (˚C)</t>
-  </si>
-  <si>
     <t>Datafiles</t>
   </si>
   <si>
@@ -93,6 +75,24 @@
   </si>
   <si>
     <t>S6_DSC.xlsx</t>
+  </si>
+  <si>
+    <t>wt</t>
+  </si>
+  <si>
+    <t>Onset Temp</t>
+  </si>
+  <si>
+    <t>Weight Loss</t>
+  </si>
+  <si>
+    <t>DTG</t>
+  </si>
+  <si>
+    <t>Non-Volatile Residue</t>
+  </si>
+  <si>
+    <t>Glass Transition Temp</t>
   </si>
 </sst>
 </file>
@@ -447,7 +447,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -467,30 +467,30 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -511,12 +511,12 @@
         <v>94.2</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -537,12 +537,12 @@
         <v>96.2</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -563,12 +563,12 @@
         <v>96.9</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -589,12 +589,12 @@
         <v>98</v>
       </c>
       <c r="H5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>15</v>
@@ -615,12 +615,12 @@
         <v>98.6</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>30</v>
@@ -641,7 +641,7 @@
         <v>99.5</v>
       </c>
       <c r="H7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalized Python code and SUBMISSION folders
</commit_message>
<xml_diff>
--- a/in-progress/Bera_2011_TActa/Bera_2011_TActa_Tidy_Table.xlsx
+++ b/in-progress/Bera_2011_TActa/Bera_2011_TActa_Tidy_Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harrisondavis/Documents/GitHub/nmcuration/in-progress/Bera_2011_TActa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDCFB88-4F6C-A64C-AF1B-105398D4200C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5793CCC-4740-C24D-BB14-D1312ECECABB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="21840" windowHeight="17540" xr2:uid="{30166B8E-BF36-4C4B-B61F-0D57A7E70461}"/>
   </bookViews>
@@ -447,7 +447,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -492,9 +492,6 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
       <c r="C2">
         <v>392</v>
       </c>
@@ -519,7 +516,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>0.02</v>
       </c>
       <c r="C3">
         <v>394.9</v>
@@ -545,7 +542,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>0.05</v>
       </c>
       <c r="C4">
         <v>395.3</v>
@@ -571,7 +568,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="C5">
         <v>397.8</v>
@@ -597,7 +594,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="C6">
         <v>401.2</v>
@@ -623,7 +620,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="C7">
         <v>396.3</v>

</xml_diff>